<commit_message>
Change template instr to English #117
</commit_message>
<xml_diff>
--- a/AdventureDayBackend/team-import/AzureAdventureDay_AzurePreparation_Template.xlsx
+++ b/AdventureDayBackend/team-import/AzureAdventureDay_AzurePreparation_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23422"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\aad\azure-adventure-day-coach\AdventureDayBackend\team-import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAB857E-BAFB-4934-9221-F3401FE36BCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E107957-6A0B-4C9E-84EB-8362D72F0895}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{DF4170B5-E2A5-144B-A2D4-E5B987ACA9B2}"/>
+    <workbookView xWindow="-13485" yWindow="5055" windowWidth="27600" windowHeight="13275" xr2:uid="{DF4170B5-E2A5-144B-A2D4-E5B987ACA9B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>Admin/Teamname</t>
   </si>
@@ -164,89 +164,86 @@
     <t>Admin/Teamname (= Subscription Name)</t>
   </si>
   <si>
-    <t>Generell</t>
-  </si>
-  <si>
-    <t>Alle Subscriptions bekommen einen eindeutigen Namen</t>
-  </si>
-  <si>
     <t>Team: Team1, Team2, Team3</t>
   </si>
   <si>
     <t>Admin: Admin</t>
   </si>
   <si>
-    <t>Alle Accounts</t>
-  </si>
-  <si>
-    <t>bekommen eindeutige Namen</t>
-  </si>
-  <si>
     <t>Coaches: Coach01, Coach02, …</t>
   </si>
   <si>
     <t>Team Attendees: Team1A1, Team1A2, Team2A1, Team2A2, …</t>
   </si>
   <si>
-    <t>Erstellung von 6 Coach Accounts</t>
-  </si>
-  <si>
-    <t>Alle Subscriptions werden neu angelegt und sind somit komplett frisch</t>
-  </si>
-  <si>
     <t>Admin Subscription</t>
   </si>
   <si>
-    <t>diese bekommen Owner Rechte auf allen Subscriptions, inkl. der Team Subscriptions</t>
-  </si>
-  <si>
-    <t>diese bekommen Admin Rechte in allen Azure ADs</t>
-  </si>
-  <si>
-    <t>sind bereits auf allen Tenants freigeschaltet / Guest Invitation ist angenommen</t>
-  </si>
-  <si>
-    <t>Erstellung einer Admin Azure Subscription</t>
-  </si>
-  <si>
-    <t>Festlegung des Spending/Notification Limits: 200$</t>
-  </si>
-  <si>
     <t>Team Subscriptions</t>
   </si>
   <si>
-    <t>Erstellung von 12 Team Azure Subscriptions</t>
-  </si>
-  <si>
-    <t>Festlegung des Spending/Notification Limits: 100$</t>
-  </si>
-  <si>
-    <t>Erstellung von 5 Team Teilnehmer Accounts, Zuweisung als Subscription Contributor</t>
-  </si>
-  <si>
-    <t>Erstellung eines Team Service Principals, Zuweisung als Subscription Owner</t>
-  </si>
-  <si>
-    <t>Erstellung eines Admin Service Principals in der Admin Subscription (Nutzung von Multi-Tenant App)</t>
-  </si>
-  <si>
-    <t>Zuweisung als Owner in allen Subscriptions, inkl. der Team Subscriptions</t>
-  </si>
-  <si>
-    <t>Übergabe der Daten</t>
-  </si>
-  <si>
-    <t>v1 - 28.10.2020</t>
-  </si>
-  <si>
-    <t>Dieses Excel als Template nutzen und die Daten in den Reitern "Azure Subscriptions" und "User Accounts &amp; SPs" eingeben</t>
+    <t>v2 - 04.03.2021</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>All subscriptions are newly created and are therefore completely fresh</t>
+  </si>
+  <si>
+    <t>All subscriptions are given a unique name (following are samples, but always ensure that in the two tabs both team name columns are matching)</t>
+  </si>
+  <si>
+    <t>All Azure accounts</t>
+  </si>
+  <si>
+    <t>get unique names</t>
+  </si>
+  <si>
+    <t>Creation of 12 Team Azure subscriptions</t>
+  </si>
+  <si>
+    <t>Setting the spending / notification limit: $ 100</t>
+  </si>
+  <si>
+    <t>Creation of a Service Principal per team, assignment as Subscription Owner</t>
+  </si>
+  <si>
+    <t>Creation of 5 Azure accounts per team, assignment as Subscription Contributor</t>
+  </si>
+  <si>
+    <t>Creation of 1 Admin Azure Subscription</t>
+  </si>
+  <si>
+    <t>Setting the spending / notification limit: $ 200</t>
+  </si>
+  <si>
+    <t>Creation of 6 Azure acounts for the coaches</t>
+  </si>
+  <si>
+    <t>Assignment as Subscription Owner for Admin Subscription and all Team Subscriptions</t>
+  </si>
+  <si>
+    <t>Assignment as Admin in all Azure AD tenants (if custom AD tenants were created)</t>
+  </si>
+  <si>
+    <t>are already activated on all tenants / guest invitation is accepted</t>
+  </si>
+  <si>
+    <t>Creation of a Service Principal for the Admin Subscription (Usage of Multi-Tenant App feature)</t>
+  </si>
+  <si>
+    <t>Transfer of data</t>
+  </si>
+  <si>
+    <t>Use this Excel as a template and enter the data in the "Azure Subscriptions" and "User Accounts &amp; SPs" tabs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -269,12 +266,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -732,8 +723,8 @@
   </sheetPr>
   <dimension ref="A2:D35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -750,127 +741,127 @@
     </row>
     <row r="3" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -881,7 +872,7 @@
     </row>
     <row r="35" spans="1:2" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1077,7 +1068,7 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1249,4 +1240,10 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>